<commit_message>
Test cases were suplemented
</commit_message>
<xml_diff>
--- a/Calculator_test_cases/test_cases_calculator.xlsx
+++ b/Calculator_test_cases/test_cases_calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Autotest\Calculator_test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,8 +14,10 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$B$32</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Вывод сообщения об ошибке "Введено недопустимое значение"</t>
   </si>
@@ -227,6 +229,33 @@
   </si>
   <si>
     <t>Ожидаемый результат</t>
+  </si>
+  <si>
+    <t>1. Запустить калькулятор
+2. Ввести число '0'
+3. Нажать '^'
+4. Ввести число '299'
+5. Нажать '='</t>
+  </si>
+  <si>
+    <t>1. Запустить калькулятор
+2. Ввести число '16,5'
+3. Выбрать операцию '/'
+4. Ввести число '5,5'
+5. Нажать '='</t>
+  </si>
+  <si>
+    <t>1. Запустить калькулятор
+2. Ввести число '1,25'
+3. Выбрать операцию '*'
+4. Ввести число '5'
+5. Нажать '='</t>
+  </si>
+  <si>
+    <t>6.25</t>
+  </si>
+  <si>
+    <t>66,45</t>
   </si>
 </sst>
 </file>
@@ -263,11 +292,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -548,16 +581,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -573,15 +606,15 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>66.45</v>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>-745.84</v>
       </c>
     </row>
@@ -589,7 +622,7 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>-7</v>
       </c>
     </row>
@@ -597,7 +630,7 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>3</v>
       </c>
     </row>
@@ -605,7 +638,7 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>102.9</v>
       </c>
     </row>
@@ -613,7 +646,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>8</v>
       </c>
     </row>
@@ -621,7 +654,7 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-4</v>
       </c>
     </row>
@@ -629,7 +662,7 @@
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -637,160 +670,184 @@
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>-1375</v>
+        <v>5</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>16.5</v>
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-1375</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>99</v>
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
+        <v>16.5</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>3.3333333333000001</v>
+        <v>4</v>
+      </c>
+      <c r="B16" s="3">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3.3332999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B20" s="3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>3.3911649916000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="3">
+        <v>3.3912</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B25" s="3">
         <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>-243</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>0.125</v>
+        <v>23</v>
+      </c>
+      <c r="B26" s="3">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>6.5536000000000003</v>
+        <v>24</v>
+      </c>
+      <c r="B27" s="3">
+        <v>-243</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>7.3003999999999998</v>
+        <v>25</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.125</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <v>6.5536000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3">
+        <v>7.3003999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B31" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>